<commit_message>
added two new pub books by beatrice potter and testing the images and paragraphs.
</commit_message>
<xml_diff>
--- a/Example/Example/Sample eBooks/BooksLibrary.xlsx
+++ b/Example/Example/Sample eBooks/BooksLibrary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>HTML</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>The Woodpeckers</t>
+  </si>
+  <si>
+    <t>The Tailor of Gloucester</t>
+  </si>
+  <si>
+    <t>The Tale of Johnny Town-Mouse</t>
+  </si>
+  <si>
+    <t>http://www.gutenberg.org/ebooks/15284</t>
+  </si>
+  <si>
+    <t>http://www.gutenberg.org/ebooks/14868</t>
   </si>
 </sst>
 </file>
@@ -576,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,210 +625,232 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new Beatrix Potter books to test on the EpubStoryReader
</commit_message>
<xml_diff>
--- a/Example/Example/Sample eBooks/BooksLibrary.xlsx
+++ b/Example/Example/Sample eBooks/BooksLibrary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
   <si>
     <t>HTML</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Poems On Travel</t>
   </si>
   <si>
-    <t>The Tale fF Peter Rabbit</t>
-  </si>
-  <si>
     <t>The Silver Chair</t>
   </si>
   <si>
@@ -220,16 +217,84 @@
   </si>
   <si>
     <t>http://www.gutenberg.org/ebooks/14868</t>
+  </si>
+  <si>
+    <t>The Tale of Two Bad Mice</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/45264</t>
+  </si>
+  <si>
+    <t>The Tale of the Pie and the Patty Pan</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/15234</t>
+  </si>
+  <si>
+    <t>The Tale of Mrs. Tittlemouse</t>
+  </si>
+  <si>
+    <t>The Tale of Mrs. Tiggy-Winkle</t>
+  </si>
+  <si>
+    <t>The Tale of Ginger and Pickles</t>
+  </si>
+  <si>
+    <t>The Story of Miss Moppet</t>
+  </si>
+  <si>
+    <t>The Story of a Fierce Bad Rabbit</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/17089</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/15137</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/14877</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/14848</t>
+  </si>
+  <si>
+    <t>The Tale of Peter Rabbit</t>
+  </si>
+  <si>
+    <t>https://www.gutenberg.org/ebooks/45265</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,13 +317,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -588,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -614,7 +712,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -625,29 +723,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -656,202 +754,279 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+    <row r="7" spans="1:3" s="1" customFormat="1">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more books in the BookLibrary
</commit_message>
<xml_diff>
--- a/Example/Example/Sample eBooks/BooksLibrary.xlsx
+++ b/Example/Example/Sample eBooks/BooksLibrary.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="25360" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EpubBooks" sheetId="1" r:id="rId1"/>
+    <sheet name="People to test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>HTML</t>
   </si>
@@ -262,6 +263,15 @@
   </si>
   <si>
     <t>https://www.gutenberg.org/ebooks/45265</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Jai</t>
   </si>
 </sst>
 </file>
@@ -688,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -1037,4 +1047,42 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>